<commit_message>
Update journal and BOM
</commit_message>
<xml_diff>
--- a/doc/BOM.xlsx
+++ b/doc/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>Nome</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Resistenza</t>
   </si>
   <si>
-    <t>TL071</t>
-  </si>
-  <si>
     <t>Microchip</t>
   </si>
   <si>
@@ -140,16 +137,13 @@
     <t>DE-DP14112V201</t>
   </si>
   <si>
-    <t>Trimmer 25K</t>
-  </si>
-  <si>
-    <t>164-34-468</t>
-  </si>
-  <si>
-    <t>67WR25KLF</t>
-  </si>
-  <si>
-    <t>BI Technologies</t>
+    <t>AD826AN</t>
+  </si>
+  <si>
+    <t>Analog Devices</t>
+  </si>
+  <si>
+    <t>173-22-437</t>
   </si>
 </sst>
 </file>
@@ -535,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H162"/>
+  <dimension ref="A1:H161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -550,7 +544,7 @@
     <col min="5" max="5" width="11.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="3" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -610,7 +604,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>16</v>
@@ -634,7 +628,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>15</v>
@@ -652,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="9">
-        <f t="shared" ref="H8:H19" si="0">G8*F8</f>
+        <f t="shared" ref="H8:H18" si="0">G8*F8</f>
         <v>0</v>
       </c>
     </row>
@@ -661,7 +655,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>22</v>
@@ -670,7 +664,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="3">
         <v>1</v>
@@ -742,26 +736,26 @@
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>8.9</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -924,43 +918,19 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="8">
-        <v>1.83</v>
-      </c>
-      <c r="H19" s="9">
-        <f t="shared" si="0"/>
-        <v>1.83</v>
-      </c>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H20" s="9"/>
+      <c r="G20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="9">
+        <f>SUM(H7:H19)</f>
+        <v>11.09</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G21" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="9">
-        <f>SUM(H7:H20)</f>
-        <v>4.0199999999999996</v>
-      </c>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H22" s="9"/>
@@ -983,9 +953,7 @@
     <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H28" s="9"/>
     </row>
-    <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H29" s="9"/>
-    </row>
+    <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1118,7 +1086,6 @@
     <row r="159" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="160" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="161" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>